<commit_message>
PB [9] - visualizar planos de nutrição
Como utilizador quero visualizar planos de nutrição
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaoc\OneDrive\Ambiente de Trabalho\Ipca_Gym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B9A501-2AB6-48E0-8DC7-65F4B1292387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1340C986-89FD-4E24-ACF2-CA2CD04FAE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="84">
   <si>
     <t>ID </t>
   </si>
@@ -128,9 +128,6 @@
     <t>quero visualizar a lotação atual do ginásio</t>
   </si>
   <si>
-    <t>quero visualizar planos de treino</t>
-  </si>
-  <si>
     <t>quero visualizar planos de nutrição</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>quero gerir a minha conta</t>
   </si>
   <si>
-    <t>quero efetuar uma compra online</t>
-  </si>
-  <si>
     <t>quero gerir a lotação no ginásio</t>
   </si>
   <si>
@@ -267,6 +261,33 @@
   </si>
   <si>
     <t>Localização</t>
+  </si>
+  <si>
+    <t>Post ou Patch em ClassificacaoController</t>
+  </si>
+  <si>
+    <t>quero efetuar recuperar a minha password</t>
+  </si>
+  <si>
+    <t>Patch em ClienteController</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>1h30</t>
+  </si>
+  <si>
+    <t>quero visualizar planos de treino (no ginásio dele)</t>
+  </si>
+  <si>
+    <t>GetAllByGinasioID em PlanoTreinoController</t>
+  </si>
+  <si>
+    <t>GetAllByGinasioID em PlanoNutricionalController</t>
   </si>
 </sst>
 </file>
@@ -553,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -708,11 +729,17 @@
     <xf numFmtId="0" fontId="10" fillId="19" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,17 +1027,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
@@ -1019,7 +1046,7 @@
     <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" customWidth="1"/>
-    <col min="12" max="12" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="50.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1054,10 +1081,10 @@
         <v>10</v>
       </c>
       <c r="K1" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="55" t="s">
-        <v>76</v>
+        <v>39</v>
+      </c>
+      <c r="L1" s="54" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1074,7 +1101,7 @@
       <c r="I2" s="43"/>
       <c r="J2" s="43"/>
       <c r="K2" s="43"/>
-      <c r="L2" s="55"/>
+      <c r="L2" s="54"/>
     </row>
     <row r="3" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="43"/>
@@ -1088,7 +1115,7 @@
       <c r="I3" s="43"/>
       <c r="J3" s="43"/>
       <c r="K3" s="43"/>
-      <c r="L3" s="55"/>
+      <c r="L3" s="54"/>
     </row>
     <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
@@ -1103,8 +1130,8 @@
       <c r="D4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>13</v>
+      <c r="E4" s="16">
+        <v>5</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>13</v>
@@ -1113,7 +1140,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>14</v>
@@ -1122,9 +1149,9 @@
         <v>13</v>
       </c>
       <c r="K4" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L4" s="57"/>
     </row>
     <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
@@ -1133,34 +1160,36 @@
       <c r="B5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="54"/>
+      <c r="D5" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="52">
+        <v>4</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="52">
+        <v>14</v>
+      </c>
+      <c r="K5" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="56" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
@@ -1170,34 +1199,34 @@
         <v>11</v>
       </c>
       <c r="C6" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="52">
+        <v>3</v>
+      </c>
+      <c r="F6" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="52">
-        <v>2</v>
-      </c>
-      <c r="F6" s="52" t="s">
+      <c r="G6" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="52">
+        <v>14</v>
+      </c>
+      <c r="K6" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="55" t="s">
         <v>73</v>
-      </c>
-      <c r="G6" s="52" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="52">
-        <v>14</v>
-      </c>
-      <c r="K6" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="51" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -1213,8 +1242,8 @@
       <c r="D7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>13</v>
+      <c r="E7" s="16">
+        <v>4</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>13</v>
@@ -1223,7 +1252,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>14</v>
@@ -1232,9 +1261,9 @@
         <v>13</v>
       </c>
       <c r="K7" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L7" s="57"/>
     </row>
     <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
@@ -1247,31 +1276,31 @@
         <v>26</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="E8" s="52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G8" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="52">
+        <v>14</v>
+      </c>
+      <c r="K8" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="55" t="s">
         <v>72</v>
-      </c>
-      <c r="H8" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="I8" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8" s="52">
-        <v>14</v>
-      </c>
-      <c r="K8" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="51" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
@@ -1281,34 +1310,36 @@
       <c r="B9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="54"/>
+      <c r="D9" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="52">
+        <v>2</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="52">
+        <v>14</v>
+      </c>
+      <c r="K9" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="56" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
@@ -1321,10 +1352,10 @@
         <v>29</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>13</v>
+        <v>53</v>
+      </c>
+      <c r="E10" s="16">
+        <v>3</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>13</v>
@@ -1333,7 +1364,7 @@
         <v>13</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>14</v>
@@ -1342,9 +1373,9 @@
         <v>13</v>
       </c>
       <c r="K10" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L10" s="57"/>
     </row>
     <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
@@ -1353,34 +1384,36 @@
       <c r="B11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" s="54"/>
+      <c r="C11" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="52">
+        <v>3</v>
+      </c>
+      <c r="F11" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" s="52">
+        <v>14</v>
+      </c>
+      <c r="K11" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="56" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
@@ -1389,34 +1422,36 @@
       <c r="B12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" s="54"/>
+      <c r="C12" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="52">
+        <v>3</v>
+      </c>
+      <c r="F12" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="56" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
@@ -1426,13 +1461,13 @@
         <v>11</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>13</v>
+      <c r="E13" s="16">
+        <v>4</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>13</v>
@@ -1441,7 +1476,7 @@
         <v>13</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I13" s="13" t="s">
         <v>14</v>
@@ -1450,25 +1485,25 @@
         <v>13</v>
       </c>
       <c r="K13" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L13" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L13" s="57"/>
     </row>
     <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>13</v>
+      <c r="E14" s="16">
+        <v>3</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>13</v>
@@ -1477,7 +1512,7 @@
         <v>13</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I14" s="13" t="s">
         <v>14</v>
@@ -1486,19 +1521,19 @@
         <v>13</v>
       </c>
       <c r="K14" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L14" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L14" s="57"/>
     </row>
     <row r="15" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="17">
-        <v>12</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>11</v>
+      <c r="A15" s="13">
+        <v>13</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>15</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>12</v>
@@ -1522,19 +1557,19 @@
         <v>13</v>
       </c>
       <c r="K15" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L15" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L15" s="57"/>
     </row>
     <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
-        <v>13</v>
+      <c r="A16" s="17">
+        <v>14</v>
       </c>
       <c r="B16" s="20" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>12</v>
@@ -1549,7 +1584,7 @@
         <v>13</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I16" s="13" t="s">
         <v>14</v>
@@ -1558,19 +1593,19 @@
         <v>13</v>
       </c>
       <c r="K16" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L16" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L16" s="57"/>
     </row>
     <row r="17" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>12</v>
@@ -1585,7 +1620,7 @@
         <v>13</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I17" s="13" t="s">
         <v>14</v>
@@ -1594,19 +1629,19 @@
         <v>13</v>
       </c>
       <c r="K17" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L17" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L17" s="57"/>
     </row>
     <row r="18" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="17">
-        <v>15</v>
+      <c r="A18" s="13">
+        <v>16</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>12</v>
@@ -1621,7 +1656,7 @@
         <v>13</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I18" s="13" t="s">
         <v>14</v>
@@ -1630,19 +1665,19 @@
         <v>13</v>
       </c>
       <c r="K18" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L18" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L18" s="57"/>
     </row>
     <row r="19" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="13">
-        <v>16</v>
-      </c>
-      <c r="B19" s="20" t="s">
+      <c r="A19" s="17">
+        <v>17</v>
+      </c>
+      <c r="B19" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>12</v>
@@ -1657,7 +1692,7 @@
         <v>13</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>14</v>
@@ -1666,19 +1701,19 @@
         <v>13</v>
       </c>
       <c r="K19" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L19" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L19" s="57"/>
     </row>
     <row r="20" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="17">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>12</v>
@@ -1693,7 +1728,7 @@
         <v>13</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I20" s="13" t="s">
         <v>14</v>
@@ -1702,19 +1737,19 @@
         <v>13</v>
       </c>
       <c r="K20" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L20" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L20" s="57"/>
     </row>
     <row r="21" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="17">
-        <v>18</v>
+      <c r="A21" s="13">
+        <v>19</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>12</v>
@@ -1729,7 +1764,7 @@
         <v>13</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I21" s="13" t="s">
         <v>14</v>
@@ -1738,13 +1773,13 @@
         <v>13</v>
       </c>
       <c r="K21" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L21" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L21" s="57"/>
     </row>
     <row r="22" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="13">
-        <v>19</v>
+      <c r="A22" s="17">
+        <v>20</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>15</v>
@@ -1765,7 +1800,7 @@
         <v>13</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I22" s="13" t="s">
         <v>14</v>
@@ -1774,19 +1809,19 @@
         <v>13</v>
       </c>
       <c r="K22" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L22" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L22" s="57"/>
     </row>
     <row r="23" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>12</v>
@@ -1801,7 +1836,7 @@
         <v>13</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I23" s="13" t="s">
         <v>14</v>
@@ -1810,19 +1845,19 @@
         <v>13</v>
       </c>
       <c r="K23" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L23" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L23" s="57"/>
     </row>
     <row r="24" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="17">
-        <v>21</v>
+      <c r="A24" s="13">
+        <v>22</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>12</v>
@@ -1837,7 +1872,7 @@
         <v>13</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I24" s="13" t="s">
         <v>14</v>
@@ -1846,19 +1881,19 @@
         <v>13</v>
       </c>
       <c r="K24" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L24" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L24" s="57"/>
     </row>
     <row r="25" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="13">
-        <v>22</v>
+      <c r="A25" s="17">
+        <v>23</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>12</v>
@@ -1873,7 +1908,7 @@
         <v>13</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I25" s="13" t="s">
         <v>14</v>
@@ -1882,19 +1917,19 @@
         <v>13</v>
       </c>
       <c r="K25" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L25" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L25" s="57"/>
     </row>
     <row r="26" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="17">
-        <v>23</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>21</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>12</v>
@@ -1909,7 +1944,7 @@
         <v>13</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I26" s="13" t="s">
         <v>14</v>
@@ -1918,13 +1953,13 @@
         <v>13</v>
       </c>
       <c r="K26" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L26" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L26" s="57"/>
     </row>
     <row r="27" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="17">
-        <v>24</v>
+      <c r="A27" s="13">
+        <v>25</v>
       </c>
       <c r="B27" s="22" t="s">
         <v>21</v>
@@ -1945,7 +1980,7 @@
         <v>13</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I27" s="13" t="s">
         <v>14</v>
@@ -1954,19 +1989,19 @@
         <v>13</v>
       </c>
       <c r="K27" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L27" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L27" s="57"/>
     </row>
     <row r="28" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="13">
-        <v>25</v>
+      <c r="A28" s="17">
+        <v>26</v>
       </c>
       <c r="B28" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>12</v>
@@ -1981,7 +2016,7 @@
         <v>13</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>14</v>
@@ -1990,19 +2025,19 @@
         <v>13</v>
       </c>
       <c r="K28" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L28" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L28" s="57"/>
     </row>
     <row r="29" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="17">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>12</v>
@@ -2017,7 +2052,7 @@
         <v>13</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I29" s="13" t="s">
         <v>14</v>
@@ -2026,19 +2061,19 @@
         <v>13</v>
       </c>
       <c r="K29" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L29" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L29" s="57"/>
     </row>
     <row r="30" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="17">
-        <v>27</v>
+      <c r="A30" s="13">
+        <v>28</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>12</v>
@@ -2053,7 +2088,7 @@
         <v>13</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>14</v>
@@ -2062,19 +2097,19 @@
         <v>13</v>
       </c>
       <c r="K30" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L30" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L30" s="57"/>
     </row>
     <row r="31" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="13">
-        <v>28</v>
+      <c r="A31" s="17">
+        <v>29</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>12</v>
@@ -2089,7 +2124,7 @@
         <v>13</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I31" s="13" t="s">
         <v>14</v>
@@ -2098,19 +2133,19 @@
         <v>13</v>
       </c>
       <c r="K31" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L31" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L31" s="57"/>
     </row>
     <row r="32" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="17">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>12</v>
@@ -2125,7 +2160,7 @@
         <v>13</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I32" s="13" t="s">
         <v>14</v>
@@ -2134,19 +2169,19 @@
         <v>13</v>
       </c>
       <c r="K32" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L32" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L32" s="57"/>
     </row>
     <row r="33" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="17">
-        <v>30</v>
+      <c r="A33" s="13">
+        <v>31</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="18" t="s">
-        <v>40</v>
+      <c r="C33" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>12</v>
@@ -2161,7 +2196,7 @@
         <v>13</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I33" s="13" t="s">
         <v>14</v>
@@ -2170,19 +2205,19 @@
         <v>13</v>
       </c>
       <c r="K33" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L33" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L33" s="57"/>
     </row>
     <row r="34" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="13">
-        <v>31</v>
+      <c r="A34" s="17">
+        <v>32</v>
       </c>
       <c r="B34" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="15" t="s">
-        <v>16</v>
+      <c r="C34" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>12</v>
@@ -2197,7 +2232,7 @@
         <v>13</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I34" s="13" t="s">
         <v>14</v>
@@ -2206,19 +2241,19 @@
         <v>13</v>
       </c>
       <c r="K34" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L34" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L34" s="57"/>
     </row>
     <row r="35" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="17">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>12</v>
@@ -2233,7 +2268,7 @@
         <v>13</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I35" s="13" t="s">
         <v>14</v>
@@ -2242,19 +2277,19 @@
         <v>13</v>
       </c>
       <c r="K35" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L35" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L35" s="57"/>
     </row>
     <row r="36" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="17">
-        <v>33</v>
+      <c r="A36" s="13">
+        <v>34</v>
       </c>
       <c r="B36" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>12</v>
@@ -2269,7 +2304,7 @@
         <v>13</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I36" s="13" t="s">
         <v>14</v>
@@ -2278,19 +2313,19 @@
         <v>13</v>
       </c>
       <c r="K36" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L36" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L36" s="57"/>
     </row>
     <row r="37" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="13">
-        <v>34</v>
+      <c r="A37" s="17">
+        <v>35</v>
       </c>
       <c r="B37" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>12</v>
@@ -2305,7 +2340,7 @@
         <v>13</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I37" s="13" t="s">
         <v>14</v>
@@ -2314,19 +2349,19 @@
         <v>13</v>
       </c>
       <c r="K37" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L37" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L37" s="57"/>
     </row>
     <row r="38" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="17">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>12</v>
@@ -2341,7 +2376,7 @@
         <v>13</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I38" s="13" t="s">
         <v>14</v>
@@ -2350,19 +2385,19 @@
         <v>13</v>
       </c>
       <c r="K38" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L38" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L38" s="57"/>
     </row>
     <row r="39" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="17">
-        <v>36</v>
+      <c r="A39" s="13">
+        <v>37</v>
       </c>
       <c r="B39" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D39" s="13" t="s">
         <v>12</v>
@@ -2377,7 +2412,7 @@
         <v>13</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I39" s="13" t="s">
         <v>14</v>
@@ -2386,19 +2421,19 @@
         <v>13</v>
       </c>
       <c r="K39" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L39" s="54"/>
+        <v>40</v>
+      </c>
+      <c r="L39" s="57"/>
     </row>
     <row r="40" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="13">
-        <v>37</v>
+      <c r="A40" s="17">
+        <v>38</v>
       </c>
       <c r="B40" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D40" s="13" t="s">
         <v>12</v>
@@ -2413,7 +2448,7 @@
         <v>13</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I40" s="13" t="s">
         <v>14</v>
@@ -2422,99 +2457,98 @@
         <v>13</v>
       </c>
       <c r="K40" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="L40" s="57"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="23"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+    </row>
+    <row r="42" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="23"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="17">
+        <v>1</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="L40" s="54"/>
-    </row>
-    <row r="41" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="17">
-        <v>38</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I41" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J41" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K41" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="L41" s="54"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="23"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-    </row>
-    <row r="43" spans="1:12" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J43" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K43" s="5" t="s">
+      <c r="I43" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" s="30" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B44" s="24" t="s">
         <v>11</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D44" s="26" t="s">
         <v>12</v>
@@ -2538,18 +2572,18 @@
         <v>13</v>
       </c>
       <c r="K44" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B45" s="24" t="s">
         <v>11</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D45" s="26" t="s">
         <v>12</v>
@@ -2564,7 +2598,7 @@
         <v>13</v>
       </c>
       <c r="H45" s="28" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I45" s="29" t="s">
         <v>14</v>
@@ -2573,56 +2607,56 @@
         <v>13</v>
       </c>
       <c r="K45" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B46" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D46" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="H46" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="I46" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J46" s="27" t="s">
+      <c r="C46" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="I46" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="33" t="s">
         <v>13</v>
       </c>
       <c r="K46" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B47" s="24" t="s">
         <v>11</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E47" s="33" t="s">
         <v>13</v>
@@ -2634,7 +2668,7 @@
         <v>13</v>
       </c>
       <c r="H47" s="34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I47" s="35" t="s">
         <v>14</v>
@@ -2643,21 +2677,21 @@
         <v>13</v>
       </c>
       <c r="K47" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B48" s="24" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E48" s="33" t="s">
         <v>13</v>
@@ -2669,7 +2703,7 @@
         <v>13</v>
       </c>
       <c r="H48" s="34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I48" s="35" t="s">
         <v>14</v>
@@ -2678,56 +2712,56 @@
         <v>13</v>
       </c>
       <c r="K48" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="17">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B49" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="D49" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="E49" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G49" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="H49" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="I49" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="J49" s="33" t="s">
+      <c r="C49" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="I49" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" s="38" t="s">
         <v>13</v>
       </c>
       <c r="K49" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B50" s="24" t="s">
         <v>11</v>
       </c>
       <c r="C50" s="36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D50" s="37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E50" s="38" t="s">
         <v>13</v>
@@ -2748,21 +2782,21 @@
         <v>13</v>
       </c>
       <c r="K50" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="17">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B51" s="24" t="s">
         <v>11</v>
       </c>
       <c r="C51" s="36" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D51" s="37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E51" s="38" t="s">
         <v>13</v>
@@ -2774,7 +2808,7 @@
         <v>13</v>
       </c>
       <c r="H51" s="39" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I51" s="40" t="s">
         <v>14</v>
@@ -2783,53 +2817,53 @@
         <v>13</v>
       </c>
       <c r="K51" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="17">
-        <v>9</v>
-      </c>
-      <c r="B52" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C52" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="D52" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="E52" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="F52" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G52" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="H52" s="39" t="s">
+      <c r="D52" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="I52" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="J52" s="38" t="s">
+      <c r="I52" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" s="27" t="s">
         <v>13</v>
       </c>
       <c r="K52" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B53" s="28" t="s">
         <v>15</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D53" s="26" t="s">
         <v>12</v>
@@ -2844,7 +2878,7 @@
         <v>13</v>
       </c>
       <c r="H53" s="28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I53" s="29" t="s">
         <v>14</v>
@@ -2853,18 +2887,18 @@
         <v>13</v>
       </c>
       <c r="K53" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="17">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B54" s="28" t="s">
         <v>15</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D54" s="26" t="s">
         <v>12</v>
@@ -2879,7 +2913,7 @@
         <v>13</v>
       </c>
       <c r="H54" s="28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I54" s="29" t="s">
         <v>14</v>
@@ -2888,56 +2922,56 @@
         <v>13</v>
       </c>
       <c r="K54" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="17">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B55" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D55" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F55" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G55" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="H55" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="I55" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J55" s="27" t="s">
+      <c r="C55" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E55" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="I55" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" s="33" t="s">
         <v>13</v>
       </c>
       <c r="K55" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="17">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B56" s="28" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E56" s="33" t="s">
         <v>13</v>
@@ -2949,7 +2983,7 @@
         <v>13</v>
       </c>
       <c r="H56" s="34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I56" s="35" t="s">
         <v>14</v>
@@ -2958,56 +2992,56 @@
         <v>13</v>
       </c>
       <c r="K56" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="17">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B57" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="D57" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="E57" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G57" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="H57" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="I57" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="J57" s="33" t="s">
+      <c r="C57" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I57" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" s="38" t="s">
         <v>13</v>
       </c>
       <c r="K57" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B58" s="28" t="s">
         <v>15</v>
       </c>
       <c r="C58" s="36" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D58" s="37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E58" s="38" t="s">
         <v>13</v>
@@ -3019,7 +3053,7 @@
         <v>13</v>
       </c>
       <c r="H58" s="39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I58" s="40" t="s">
         <v>14</v>
@@ -3028,133 +3062,115 @@
         <v>13</v>
       </c>
       <c r="K58" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="17">
-        <v>16</v>
-      </c>
-      <c r="B59" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C59" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="D59" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="E59" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="F59" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G59" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="H59" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="I59" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="J59" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E59" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="I59" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59" s="33" t="s">
         <v>13</v>
       </c>
       <c r="K59" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="17">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B60" s="41" t="s">
         <v>21</v>
       </c>
       <c r="C60" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E60" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="I60" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J60" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="K60" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="C61" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D60" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="E60" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G60" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="H60" s="34" t="s">
+    </row>
+    <row r="63" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C64" s="7"/>
+      <c r="D64" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F64" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I60" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="J60" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="K60" s="30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="17">
+    </row>
+    <row r="65" spans="3:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="C65" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D65" s="10">
+        <f>COUNTIF(H4:H40,"João")</f>
+        <v>11</v>
+      </c>
+      <c r="E65" s="10">
+        <f>COUNTIF(H43:H60,"João")</f>
+        <v>7</v>
+      </c>
+      <c r="F65" s="10">
+        <f>SUM(D65,E65)</f>
         <v>18</v>
-      </c>
-      <c r="B61" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C61" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="D61" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="E61" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="F61" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G61" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="H61" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="I61" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="J61" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="K61" s="30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-      <c r="C62" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C64" s="2"/>
-    </row>
-    <row r="65" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C65" s="7"/>
-      <c r="D65" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="66" spans="3:6" ht="15" x14ac:dyDescent="0.3">
@@ -3162,101 +3178,84 @@
         <v>64</v>
       </c>
       <c r="D66" s="10">
-        <f>COUNTIF(H4:H41,"João")</f>
-        <v>12</v>
+        <f>COUNTIF(H4:H40,"Pedro")</f>
+        <v>13</v>
       </c>
       <c r="E66" s="10">
-        <f>COUNTIF(H44:H61,"João")</f>
-        <v>7</v>
+        <f>COUNTIF(H43:H60,"Pedro")</f>
+        <v>5</v>
       </c>
       <c r="F66" s="10">
         <f>SUM(D66,E66)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="3:6" ht="15" x14ac:dyDescent="0.3">
       <c r="C67" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D67" s="10">
-        <f>COUNTIF(H4:H41,"Pedro")</f>
+        <f>COUNTIF(H4:H40,"Gonçalo")</f>
         <v>13</v>
       </c>
       <c r="E67" s="10">
-        <f>COUNTIF(H44:H61,"Pedro")</f>
-        <v>5</v>
+        <f>COUNTIF(H43:H60,"Gonçalo")</f>
+        <v>6</v>
       </c>
       <c r="F67" s="10">
         <f>SUM(D67,E67)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="C70" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D70" s="10">
+        <f>COUNTIF(I4:I40,"To Do")</f>
+        <v>31</v>
+      </c>
+      <c r="E70" s="10">
+        <f>COUNTIF(I43:I60,"To Do")</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="68" spans="3:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="C68" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D68" s="10">
-        <f>COUNTIF(H4:H41,"Gonçalo")</f>
-        <v>13</v>
-      </c>
-      <c r="E68" s="10">
-        <f>COUNTIF(H44:H61,"Gonçalo")</f>
-        <v>6</v>
-      </c>
-      <c r="F68" s="10">
-        <f>SUM(D68,E68)</f>
-        <v>19</v>
+      <c r="F70" s="10">
+        <f>SUM(E70,D70)</f>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="3:6" ht="15" x14ac:dyDescent="0.3">
       <c r="C71" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D71" s="10">
-        <f>COUNTIF(I44:I61,"To Do")</f>
-        <v>18</v>
+        <f>COUNTIF(I4:I40,"Doing")</f>
+        <v>1</v>
       </c>
       <c r="E71" s="10">
-        <f>COUNTIF(I4:I41,"To Do")</f>
-        <v>36</v>
+        <f>COUNTIF(I43:I60,"Doing")</f>
+        <v>0</v>
       </c>
       <c r="F71" s="10">
         <f>SUM(D71,E71)</f>
-        <v>54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="3:6" ht="15" x14ac:dyDescent="0.3">
       <c r="C72" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D72" s="10">
-        <f>COUNTIF(I4:I41,"Doing")</f>
+        <f>COUNTIF(I4:I40,"Done")</f>
+        <v>5</v>
+      </c>
+      <c r="E72" s="10">
+        <f>COUNTIF(I43:I60,"Done")</f>
         <v>0</v>
       </c>
-      <c r="E72" s="10">
-        <f>COUNTIF(I44:I61,"Doing")</f>
-        <v>0</v>
-      </c>
       <c r="F72" s="10">
-        <f>SUM(D72,E72)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="3:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="C73" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D73" s="10">
-        <f>COUNTIF(I44:I61,"Done")</f>
-        <v>0</v>
-      </c>
-      <c r="E73" s="10">
-        <f>COUNTIF(I4:I41,"Done")</f>
-        <v>2</v>
-      </c>
-      <c r="F73" s="10">
-        <f>SUM(D73,E73)</f>
-        <v>2</v>
+        <f>SUM(E72,D72)</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Product Backlog Excel
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaoc\OneDrive\Ambiente de Trabalho\Ipca_Gym\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonçalo Cunha\Desktop\Universidade\ipca_gym\ipca_gym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2294DD-F3EB-421D-A07C-AD6EF58B2409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA819F1-ABB9-4E05-9360-CFC4F41B9F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="121">
   <si>
     <t>ID </t>
   </si>
@@ -336,13 +336,79 @@
     <t>Quantidade -&gt; PatchPedidoChecked em PedidoLojaController
 Add Produto -&gt; PostPedidoChecked em PedidoLojaController
 Rem Produto -&gt; DeletePedido em PedidoLojaController</t>
+  </si>
+  <si>
+    <t>Patch em FuncionarioController</t>
+  </si>
+  <si>
+    <t>quero visualizar as avaliações do ginásio</t>
+  </si>
+  <si>
+    <t>Patch GinasioController</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1H</t>
+  </si>
+  <si>
+    <t>GetAllConectionCliente em PedidoController</t>
+  </si>
+  <si>
+    <t>quero visualizar a lotação no ginásio</t>
+  </si>
+  <si>
+    <t>Get GinasioController</t>
+  </si>
+  <si>
+    <t>Patch FuncionarioController</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Post em HorarioFuncionarioController</t>
+  </si>
+  <si>
+    <t>Patch em HorarioFuncionarioController</t>
+  </si>
+  <si>
+    <t>Delete em HorarioFuncionarioController</t>
+  </si>
+  <si>
+    <t>Post em ClienteController</t>
+  </si>
+  <si>
+    <t>Post em FuncionarioController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quero apagar um cliente </t>
+  </si>
+  <si>
+    <t>20min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quero cirar um horario </t>
+  </si>
+  <si>
+    <t xml:space="preserve">quero editar um horario </t>
+  </si>
+  <si>
+    <t xml:space="preserve">quero remover um horario </t>
+  </si>
+  <si>
+    <t xml:space="preserve">quero visualizar um horario </t>
+  </si>
+  <si>
+    <t>Get em HorarioFuncionarioController</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,6 +480,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="19">
@@ -616,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -730,10 +804,46 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -748,42 +858,40 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1070,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L76"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1094,72 +1202,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="53" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="52" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="42"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="39"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="52"/>
     </row>
     <row r="3" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="43"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="55"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="39"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="52"/>
     </row>
     <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
@@ -1239,7 +1347,7 @@
       <c r="A6" s="16">
         <v>3</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="43" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -1277,7 +1385,7 @@
       <c r="A7" s="12">
         <v>4</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="43" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="22" t="s">
@@ -1307,7 +1415,7 @@
       <c r="K7" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="56" t="s">
+      <c r="L7" s="48" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1315,43 +1423,45 @@
       <c r="A8" s="16">
         <v>5</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="26">
         <v>3</v>
       </c>
-      <c r="F8" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="33" t="s">
+      <c r="F8" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="33" t="s">
+      <c r="I8" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" s="35"/>
+      <c r="J8" s="26">
+        <v>15</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="29" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="90" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>6</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="43" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="22" t="s">
@@ -1381,7 +1491,7 @@
       <c r="K9" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="56" t="s">
+      <c r="L9" s="48" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1389,7 +1499,7 @@
       <c r="A10" s="12">
         <v>7</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="43" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -1427,7 +1537,7 @@
       <c r="A11" s="16">
         <v>8</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="43" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="22" t="s">
@@ -1465,7 +1575,7 @@
       <c r="A12" s="16">
         <v>9</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="43" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="22" t="s">
@@ -1503,7 +1613,7 @@
       <c r="A13" s="12">
         <v>10</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="43" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="22" t="s">
@@ -1541,7 +1651,7 @@
       <c r="A14" s="16">
         <v>12</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="43" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="22" t="s">
@@ -1579,10 +1689,10 @@
       <c r="A15" s="12">
         <v>13</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="39" t="s">
         <v>83</v>
       </c>
       <c r="D15" s="12" t="s">
@@ -1615,10 +1725,10 @@
       <c r="A16" s="16">
         <v>14</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="39" t="s">
         <v>85</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -1647,14 +1757,14 @@
       </c>
       <c r="L16" s="30"/>
     </row>
-    <row r="17" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>15</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="39" t="s">
         <v>84</v>
       </c>
       <c r="D17" s="12" t="s">
@@ -1683,14 +1793,14 @@
       </c>
       <c r="L17" s="30"/>
     </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>16</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="44" t="s">
         <v>75</v>
       </c>
       <c r="D18" s="32" t="s">
@@ -1719,7 +1829,7 @@
       </c>
       <c r="L18" s="35"/>
     </row>
-    <row r="19" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
         <v>17</v>
       </c>
@@ -1757,14 +1867,14 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
         <v>18</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="36" t="s">
@@ -1795,7 +1905,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>19</v>
       </c>
@@ -1831,7 +1941,7 @@
       </c>
       <c r="L21" s="30"/>
     </row>
-    <row r="22" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="16">
         <v>20</v>
       </c>
@@ -1867,11 +1977,11 @@
       </c>
       <c r="L22" s="30"/>
     </row>
-    <row r="23" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="16">
         <v>21</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="46" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="22" t="s">
@@ -1903,14 +2013,14 @@
       </c>
       <c r="L23" s="30"/>
     </row>
-    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>22</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="39" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="12" t="s">
@@ -1939,11 +2049,11 @@
       </c>
       <c r="L24" s="30"/>
     </row>
-    <row r="25" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
         <v>23</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="46" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="22" t="s">
@@ -1975,14 +2085,14 @@
       </c>
       <c r="L25" s="30"/>
     </row>
-    <row r="26" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="16">
         <v>24</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="47" t="s">
+      <c r="C26" s="39" t="s">
         <v>32</v>
       </c>
       <c r="D26" s="12" t="s">
@@ -2011,14 +2121,14 @@
       </c>
       <c r="L26" s="30"/>
     </row>
-    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>25</v>
       </c>
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="39" t="s">
         <v>33</v>
       </c>
       <c r="D27" s="12" t="s">
@@ -2047,14 +2157,14 @@
       </c>
       <c r="L27" s="30"/>
     </row>
-    <row r="28" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <v>26</v>
       </c>
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="39" t="s">
         <v>34</v>
       </c>
       <c r="D28" s="12" t="s">
@@ -2083,14 +2193,14 @@
       </c>
       <c r="L28" s="30"/>
     </row>
-    <row r="29" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="16">
         <v>27</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="39" t="s">
         <v>35</v>
       </c>
       <c r="D29" s="12" t="s">
@@ -2119,1191 +2229,1244 @@
       </c>
       <c r="L29" s="30"/>
     </row>
-    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>28</v>
       </c>
-      <c r="B30" s="55" t="s">
+      <c r="B30" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H30" s="15" t="s">
+      <c r="D30" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="37">
+        <v>4</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="I30" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K30" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L30" s="30"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I30" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J30" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="L30" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="P30" s="68"/>
+    </row>
+    <row r="31" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="16">
         <v>29</v>
       </c>
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="15" t="s">
+      <c r="C31" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="37">
+        <v>3</v>
+      </c>
+      <c r="F31" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="I31" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J31" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K31" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L31" s="30"/>
-    </row>
-    <row r="32" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I31" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J31" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="K31" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="L31" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="16">
         <v>30</v>
       </c>
-      <c r="B32" s="55" t="s">
+      <c r="B32" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="15" t="s">
+      <c r="D32" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="37">
+        <v>3</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="I32" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K32" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L32" s="30"/>
-    </row>
-    <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="I32" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J32" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="L32" s="29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>31</v>
       </c>
-      <c r="B33" s="55" t="s">
+      <c r="B33" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="15" t="s">
+      <c r="C33" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="63">
+        <v>2</v>
+      </c>
+      <c r="F33" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="I33" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J33" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K33" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L33" s="30"/>
-    </row>
-    <row r="34" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I33" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="J33" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33" s="35"/>
+      <c r="M33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="16">
         <v>32</v>
       </c>
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" s="15" t="s">
+      <c r="D34" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="I34" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J34" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K34" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L34" s="30"/>
-    </row>
-    <row r="35" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I34" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="L34" s="61"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="16">
         <v>33</v>
       </c>
-      <c r="B35" s="55" t="s">
+      <c r="B35" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="15" t="s">
+      <c r="D35" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="63">
+        <v>4</v>
+      </c>
+      <c r="F35" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="I35" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K35" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L35" s="30"/>
-    </row>
-    <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="I35" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="J35" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="L35" s="35"/>
+      <c r="M35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>34</v>
       </c>
-      <c r="B36" s="55" t="s">
+      <c r="B36" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="15" t="s">
+      <c r="D36" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="26">
+        <v>4</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H36" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="I36" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J36" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K36" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L36" s="30"/>
-    </row>
-    <row r="37" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I36" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J36" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L36" s="29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="16">
         <v>35</v>
       </c>
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="15" t="s">
+      <c r="D37" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="G37" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H37" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="I37" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J37" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K37" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L37" s="30"/>
-    </row>
-    <row r="38" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I37" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J37" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L37" s="29"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="16">
         <v>36</v>
       </c>
-      <c r="B38" s="55" t="s">
+      <c r="B38" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="47" t="s">
+      <c r="C38" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" s="15" t="s">
+      <c r="D38" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H38" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="I38" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K38" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L38" s="30"/>
-    </row>
-    <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="I38" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J38" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L38" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
         <v>37</v>
       </c>
-      <c r="B39" s="55" t="s">
+      <c r="B39" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C39" s="47" t="s">
+      <c r="C39" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="15" t="s">
+      <c r="D39" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="26">
+        <v>4</v>
+      </c>
+      <c r="F39" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G39" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H39" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="I39" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J39" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K39" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L39" s="30"/>
-    </row>
-    <row r="40" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I39" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J39" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K39" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L39" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="16">
         <v>38</v>
       </c>
-      <c r="B40" s="55" t="s">
+      <c r="B40" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="15" t="s">
+      <c r="D40" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="I40" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J40" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K40" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L40" s="30"/>
-    </row>
-    <row r="41" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I40" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="L40" s="61"/>
+      <c r="M40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="16">
         <v>39</v>
       </c>
-      <c r="B41" s="55" t="s">
+      <c r="B41" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="47" t="s">
+      <c r="C41" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="15" t="s">
+      <c r="D41" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="26">
+        <v>5</v>
+      </c>
+      <c r="F41" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G41" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="I41" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J41" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K41" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L41" s="30"/>
-    </row>
-    <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="I41" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J41" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K41" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L41" s="29"/>
+    </row>
+    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A42" s="12">
         <v>40</v>
       </c>
-      <c r="B42" s="55" t="s">
+      <c r="B42" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="47" t="s">
+      <c r="C42" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="15" t="s">
+      <c r="D42" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F42" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G42" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H42" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="I42" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J42" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K42" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L42" s="30"/>
-    </row>
-    <row r="43" spans="1:12" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="55" t="s">
+      <c r="I42" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J42" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L42" s="29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="16">
+        <v>41</v>
+      </c>
+      <c r="B43" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="47" t="s">
+      <c r="C43" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="15" t="s">
+      <c r="D43" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="26">
+        <v>5</v>
+      </c>
+      <c r="F43" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H43" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="I43" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J43" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K43" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L43" s="30"/>
-    </row>
-    <row r="44" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I43" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J43" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L43" s="29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="16">
+        <v>42</v>
+      </c>
+      <c r="B44" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="59">
+        <v>4</v>
+      </c>
+      <c r="F44" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="I44" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="K44" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="L44" s="61"/>
+      <c r="M44">
         <v>1</v>
       </c>
-      <c r="B44" s="55" t="s">
+    </row>
+    <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A45" s="12">
+        <v>43</v>
+      </c>
+      <c r="B45" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="15" t="s">
+      <c r="C45" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="26">
+        <v>5</v>
+      </c>
+      <c r="F45" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G45" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H45" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="I44" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K44" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L44" s="30"/>
-    </row>
-    <row r="45" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="16">
+      <c r="I45" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J45" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K45" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L45" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="N45" s="68"/>
+    </row>
+    <row r="46" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="16">
+        <v>44</v>
+      </c>
+      <c r="B46" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="26">
+        <v>5</v>
+      </c>
+      <c r="F46" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G46" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H46" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="I46" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J46" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K46" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L46" s="48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="16">
+        <v>45</v>
+      </c>
+      <c r="B47" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="26">
+        <v>5</v>
+      </c>
+      <c r="F47" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G47" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H47" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="I47" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J47" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K47" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L47" s="48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A48" s="12">
+        <v>46</v>
+      </c>
+      <c r="B48" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="26">
+        <v>4</v>
+      </c>
+      <c r="F48" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G48" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H48" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="I48" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J48" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K48" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L48" s="48" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="16">
+        <v>47</v>
+      </c>
+      <c r="B49" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="59">
+        <v>4</v>
+      </c>
+      <c r="F49" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="I49" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="K49" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="L49" s="61"/>
+      <c r="M49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="16"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+    </row>
+    <row r="51" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="16">
+        <v>1</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="16">
         <v>2</v>
-      </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-    </row>
-    <row r="46" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="16">
-        <v>3</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="16">
-        <v>4</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="D47" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F47" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="H47" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="I47" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J47" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="K47" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="16">
-        <v>5</v>
-      </c>
-      <c r="B48" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="D48" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F48" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="G48" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="I48" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J48" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="K48" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="16">
-        <v>6</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="G49" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="H49" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="I49" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J49" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="K49" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="16">
-        <v>7</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="D50" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H50" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="I50" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J50" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K50" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="16">
-        <v>8</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="D51" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H51" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="I51" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J51" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K51" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="16">
-        <v>9</v>
       </c>
       <c r="B52" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="D52" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G52" s="15" t="s">
+      <c r="C52" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="41" t="s">
         <v>13</v>
       </c>
       <c r="H52" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I52" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J52" s="15" t="s">
+      <c r="I52" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" s="41" t="s">
         <v>13</v>
       </c>
       <c r="K52" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="16">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B53" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D53" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="E53" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" s="49" t="s">
+      <c r="C53" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="D53" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="41" t="s">
         <v>13</v>
       </c>
       <c r="H53" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="I53" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J53" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="I53" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J53" s="41" t="s">
         <v>13</v>
       </c>
       <c r="K53" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="16">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B54" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="D54" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="E54" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="G54" s="49" t="s">
+      <c r="C54" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D54" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="41" t="s">
         <v>13</v>
       </c>
       <c r="H54" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="I54" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J54" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="I54" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J54" s="41" t="s">
         <v>13</v>
       </c>
       <c r="K54" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="16">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B55" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C55" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="E55" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F55" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="G55" s="49" t="s">
+      <c r="C55" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D55" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="15" t="s">
         <v>13</v>
       </c>
       <c r="H55" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I55" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J55" s="49" t="s">
+      <c r="I55" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" s="15" t="s">
         <v>13</v>
       </c>
       <c r="K55" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="16">
-        <v>13</v>
-      </c>
-      <c r="B56" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C56" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="D56" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F56" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="G56" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D56" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56" s="15" t="s">
         <v>13</v>
       </c>
       <c r="H56" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="I56" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J56" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J56" s="15" t="s">
         <v>13</v>
       </c>
       <c r="K56" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="16">
-        <v>14</v>
-      </c>
-      <c r="B57" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C57" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="D57" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="E57" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="G57" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D57" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="15" t="s">
         <v>13</v>
       </c>
       <c r="H57" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="I57" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J57" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="I57" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" s="15" t="s">
         <v>13</v>
       </c>
       <c r="K57" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="16">
-        <v>15</v>
-      </c>
-      <c r="B58" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="D58" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F58" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="G58" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D58" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E58" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" s="41" t="s">
         <v>13</v>
       </c>
       <c r="H58" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="I58" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J58" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="I58" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J58" s="41" t="s">
         <v>13</v>
       </c>
       <c r="K58" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="16">
-        <v>16</v>
-      </c>
-      <c r="B59" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C59" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="D59" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F59" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G59" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E59" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" s="41" t="s">
         <v>13</v>
       </c>
       <c r="H59" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="I59" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J59" s="15" t="s">
+      <c r="I59" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59" s="41" t="s">
         <v>13</v>
       </c>
       <c r="K59" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="16">
-        <v>17</v>
-      </c>
-      <c r="B60" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="D60" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G60" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E60" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="41" t="s">
         <v>13</v>
       </c>
       <c r="H60" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J60" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I60" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J60" s="41" t="s">
         <v>13</v>
       </c>
       <c r="K60" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="16">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B61" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D61" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="E61" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F61" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="G61" s="49" t="s">
+      <c r="C61" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D61" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" s="41" t="s">
         <v>13</v>
       </c>
       <c r="H61" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="I61" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J61" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="I61" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J61" s="41" t="s">
         <v>13</v>
       </c>
       <c r="K61" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="16">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B62" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C62" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="D62" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="E62" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F62" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="G62" s="49" t="s">
+      <c r="C62" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D62" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="41" t="s">
         <v>13</v>
       </c>
       <c r="H62" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I62" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J62" s="49" t="s">
+      <c r="I62" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J62" s="41" t="s">
         <v>13</v>
       </c>
       <c r="K62" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B63" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C63" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="D63" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E63" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F63" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G63" s="15" t="s">
+    <row r="63" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="16">
+        <v>13</v>
+      </c>
+      <c r="B63" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D63" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="41" t="s">
         <v>13</v>
       </c>
       <c r="H63" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I63" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J63" s="15" t="s">
+      <c r="I63" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J63" s="41" t="s">
         <v>13</v>
       </c>
       <c r="K63" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B64" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C64" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D64" s="48" t="s">
+    <row r="64" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="16">
+        <v>14</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D64" s="40" t="s">
         <v>52</v>
       </c>
       <c r="E64" s="15" t="s">
@@ -3316,7 +3479,7 @@
         <v>13</v>
       </c>
       <c r="H64" s="21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I64" s="12" t="s">
         <v>14</v>
@@ -3328,141 +3491,316 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C65" s="1" t="s">
+    <row r="65" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="16">
+        <v>15</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E65" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="I65" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J65" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K65" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="16">
+        <v>16</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D66" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E66" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G66" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H66" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I66" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J66" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="K66" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="16">
+        <v>17</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E67" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F67" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H67" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I67" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J67" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="K67" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="16">
+        <v>18</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D68" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H68" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I68" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J68" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K68" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="16">
+        <v>19</v>
+      </c>
+      <c r="B69" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D69" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H69" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I69" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J69" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K69" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C70" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C68" s="6"/>
-      <c r="D68" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E68" s="7" t="s">
+    <row r="72" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C73" s="6"/>
+      <c r="D73" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E73" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F68" s="7" t="s">
+      <c r="F73" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="3:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="C69" s="8" t="s">
+    <row r="74" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="C74" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D69" s="9">
-        <f>COUNTIF(H4:H44,"João")</f>
+      <c r="D74" s="9">
+        <f>COUNTIF(H4:H49,"João")</f>
         <v>15</v>
       </c>
-      <c r="E69" s="9">
-        <f>COUNTIF(H47:H64,"João")</f>
+      <c r="E74" s="9">
+        <f>COUNTIF(H52:H69,"João")</f>
         <v>7</v>
       </c>
-      <c r="F69" s="9">
-        <f>SUM(D69,E69)</f>
+      <c r="F74" s="9">
+        <f>SUM(D74,E74)</f>
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="3:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="C70" s="8" t="s">
+    <row r="75" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="C75" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D70" s="9">
-        <f>COUNTIF(H4:H44,"Pedro")</f>
-        <v>13</v>
-      </c>
-      <c r="E70" s="9">
-        <f>COUNTIF(H47:H64,"Pedro")</f>
+      <c r="D75" s="9">
+        <f>COUNTIF(H4:H49,"Pedro")</f>
+        <v>13</v>
+      </c>
+      <c r="E75" s="9">
+        <f>COUNTIF(H52:H69,"Pedro")</f>
         <v>5</v>
-      </c>
-      <c r="F70" s="9">
-        <f>SUM(D70,E70)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71" spans="3:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="C71" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D71" s="9">
-        <f>COUNTIF(H4:H44,"Gonçalo")</f>
-        <v>13</v>
-      </c>
-      <c r="E71" s="9">
-        <f>COUNTIF(H47:H64,"Gonçalo")</f>
-        <v>6</v>
-      </c>
-      <c r="F71" s="9">
-        <f>SUM(D71,E71)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="74" spans="3:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="C74" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D74" s="9">
-        <f>COUNTIF(I4:I44,"To Do")</f>
-        <v>24</v>
-      </c>
-      <c r="E74" s="9">
-        <f>COUNTIF(I47:I64,"To Do")</f>
-        <v>18</v>
-      </c>
-      <c r="F74" s="9">
-        <f>SUM(E74,D74)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="75" spans="3:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="C75" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D75" s="9">
-        <f>COUNTIF(I4:I44,"Doing")</f>
-        <v>2</v>
-      </c>
-      <c r="E75" s="9">
-        <f>COUNTIF(I47:I64,"Doing")</f>
-        <v>0</v>
       </c>
       <c r="F75" s="9">
         <f>SUM(D75,E75)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="3:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="C76" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="C76" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D76" s="9">
+        <f>COUNTIF(H4:H49,"Gonçalo")</f>
+        <v>18</v>
+      </c>
+      <c r="E76" s="9">
+        <f>COUNTIF(H52:H69,"Gonçalo")</f>
+        <v>6</v>
+      </c>
+      <c r="F76" s="9">
+        <f>SUM(D76,E76)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="C79" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D79" s="9">
+        <f>COUNTIF(I4:I49,"To Do")</f>
+        <v>13</v>
+      </c>
+      <c r="E79" s="9">
+        <f>COUNTIF(I52:I69,"To Do")</f>
+        <v>18</v>
+      </c>
+      <c r="F79" s="9">
+        <f>SUM(E79,D79)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="C80" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D80" s="9">
+        <f>COUNTIF(I4:I49,"Doing")</f>
+        <v>4</v>
+      </c>
+      <c r="E80" s="9">
+        <f>COUNTIF(I52:I69,"Doing")</f>
+        <v>0</v>
+      </c>
+      <c r="F80" s="9">
+        <f>SUM(D80,E80)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="C81" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D76" s="9">
-        <f>COUNTIF(I4:I44,"Done")</f>
-        <v>15</v>
-      </c>
-      <c r="E76" s="9">
-        <f>COUNTIF(I47:I64,"Done")</f>
+      <c r="D81" s="9">
+        <f>COUNTIF(I4:I49,"Done")</f>
+        <v>29</v>
+      </c>
+      <c r="E81" s="9">
+        <f>COUNTIF(I52:I69,"Done")</f>
         <v>0</v>
       </c>
-      <c r="F76" s="9">
-        <f>SUM(E76,D76)</f>
-        <v>15</v>
+      <c r="F81" s="9">
+        <f>SUM(E81,D81)</f>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
     <mergeCell ref="L1:L3"/>
     <mergeCell ref="K1:K3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="H1:H3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
User case - Ver classificacoes de um ginasio + update backlog
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonçalo Cunha\Desktop\Universidade\ipca_gym\ipca_gym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA819F1-ABB9-4E05-9360-CFC4F41B9F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B795BB-E8B0-485A-B5AB-486804D04D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="123">
   <si>
     <t>ID </t>
   </si>
@@ -402,13 +402,19 @@
   </si>
   <si>
     <t>Get em HorarioFuncionarioController</t>
+  </si>
+  <si>
+    <t>1.5H</t>
+  </si>
+  <si>
+    <t>GetAllClassificationsByGinasioID em ClassificacaoController</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,6 +494,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -690,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -834,16 +846,35 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -858,40 +889,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1180,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,77 +1203,77 @@
     <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" customWidth="1"/>
-    <col min="12" max="12" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="66" customWidth="1"/>
     <col min="13" max="13" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="60" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="54"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="61"/>
       <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="56"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="52"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="58"/>
     </row>
     <row r="3" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="55"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="62"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="52"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="58"/>
     </row>
     <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
@@ -2156,6 +2162,7 @@
         <v>39</v>
       </c>
       <c r="L27" s="30"/>
+      <c r="P27" s="57"/>
     </row>
     <row r="28" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
@@ -2239,7 +2246,7 @@
       <c r="C30" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="65" t="s">
+      <c r="D30" s="54" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="37">
@@ -2260,13 +2267,13 @@
       <c r="J30" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="K30" s="66" t="s">
+      <c r="K30" s="55" t="s">
         <v>39</v>
       </c>
       <c r="L30" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="P30" s="68"/>
+      <c r="P30" s="57"/>
     </row>
     <row r="31" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="16">
@@ -2278,7 +2285,7 @@
       <c r="C31" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D31" s="65" t="s">
+      <c r="D31" s="54" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="37">
@@ -2299,7 +2306,7 @@
       <c r="J31" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="K31" s="66" t="s">
+      <c r="K31" s="55" t="s">
         <v>39</v>
       </c>
       <c r="L31" s="29" t="s">
@@ -2316,7 +2323,7 @@
       <c r="C32" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="65" t="s">
+      <c r="D32" s="54" t="s">
         <v>12</v>
       </c>
       <c r="E32" s="37">
@@ -2337,7 +2344,7 @@
       <c r="J32" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="K32" s="66" t="s">
+      <c r="K32" s="55" t="s">
         <v>39</v>
       </c>
       <c r="L32" s="29" t="s">
@@ -2351,36 +2358,35 @@
       <c r="B33" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="63">
+      <c r="D33" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="37">
         <v>2</v>
       </c>
-      <c r="F33" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="63" t="s">
+      <c r="F33" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="G33" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="I33" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="J33" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="K33" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="L33" s="35"/>
-      <c r="M33">
-        <v>1</v>
+      <c r="I33" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J33" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33" s="29" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -2390,34 +2396,34 @@
       <c r="B34" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="57" t="s">
+      <c r="C34" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" s="59" t="s">
+      <c r="D34" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="I34" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="J34" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="K34" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="L34" s="61"/>
+      <c r="I34" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="L34" s="30"/>
     </row>
     <row r="35" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="16">
@@ -2429,28 +2435,28 @@
       <c r="C35" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="63">
+      <c r="D35" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="53">
         <v>4</v>
       </c>
-      <c r="F35" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="63" t="s">
+      <c r="F35" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="53" t="s">
         <v>62</v>
       </c>
       <c r="I35" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="J35" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="K35" s="64" t="s">
+      <c r="J35" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" s="66" t="s">
         <v>39</v>
       </c>
       <c r="L35" s="35"/>
@@ -2503,7 +2509,7 @@
       <c r="B37" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="67" t="s">
+      <c r="C37" s="56" t="s">
         <v>16</v>
       </c>
       <c r="D37" s="25" t="s">
@@ -2615,34 +2621,34 @@
       <c r="B40" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="57" t="s">
+      <c r="C40" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="59" t="s">
+      <c r="D40" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="I40" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="J40" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="K40" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="L40" s="61"/>
+      <c r="I40" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="L40" s="30"/>
       <c r="M40">
         <v>1</v>
       </c>
@@ -2766,34 +2772,34 @@
       <c r="B44" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="57" t="s">
+      <c r="C44" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="59">
+      <c r="D44" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="38">
         <v>4</v>
       </c>
-      <c r="F44" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="59" t="s">
+      <c r="F44" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="I44" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="K44" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="L44" s="61"/>
+      <c r="I44" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="K44" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="L44" s="30"/>
       <c r="M44">
         <v>1</v>
       </c>
@@ -2835,7 +2841,7 @@
       <c r="L45" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="N45" s="68"/>
+      <c r="N45" s="57"/>
     </row>
     <row r="46" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="16">
@@ -2958,34 +2964,34 @@
       <c r="B49" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C49" s="57" t="s">
+      <c r="C49" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="D49" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="59">
+      <c r="D49" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="38">
         <v>4</v>
       </c>
-      <c r="F49" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="G49" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="H49" s="59" t="s">
+      <c r="F49" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="I49" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="J49" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="K49" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="L49" s="61"/>
+      <c r="I49" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="K49" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="L49" s="30"/>
       <c r="M49">
         <v>1</v>
       </c>
@@ -3760,7 +3766,7 @@
       </c>
       <c r="D80" s="9">
         <f>COUNTIF(I4:I49,"Doing")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E80" s="9">
         <f>COUNTIF(I52:I69,"Doing")</f>
@@ -3768,7 +3774,7 @@
       </c>
       <c r="F80" s="9">
         <f>SUM(D80,E80)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="3:6" ht="15" x14ac:dyDescent="0.3">
@@ -3777,7 +3783,7 @@
       </c>
       <c r="D81" s="9">
         <f>COUNTIF(I4:I49,"Done")</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E81" s="9">
         <f>COUNTIF(I52:I69,"Done")</f>
@@ -3785,22 +3791,22 @@
       </c>
       <c r="F81" s="9">
         <f>SUM(E81,D81)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
     <mergeCell ref="L1:L3"/>
     <mergeCell ref="K1:K3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="H1:H3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
PB [23] - Funcionario Editar Stock
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonçalo Cunha\Desktop\Universidade\ipca_gym\ipca_gym\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TrabalhosPraticos\Projeto_Aplicado\ipca_gym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B795BB-E8B0-485A-B5AB-486804D04D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5539879E-858F-4582-94FA-8279E661D54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="121">
   <si>
     <t>ID </t>
   </si>
@@ -297,12 +297,6 @@
   </si>
   <si>
     <t>30min</t>
-  </si>
-  <si>
-    <t>quero apagar conta de um user  NEW METHOD</t>
-  </si>
-  <si>
-    <t>quero editar os dados biométricos de um user NEW METHOD</t>
   </si>
   <si>
     <t>45min</t>
@@ -702,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -871,6 +865,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -893,9 +899,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1186,96 +1189,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="52.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="12" width="66" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:12" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="64" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="59" t="s">
+      <c r="H1" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="62" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="59"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="61"/>
+    <row r="2" spans="1:12" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="63"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="65"/>
       <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="58"/>
-    </row>
-    <row r="3" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="59"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="62"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="62"/>
+    </row>
+    <row r="3" spans="1:12" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="63"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="66"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="58"/>
-    </row>
-    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="62"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -1311,7 +1314,7 @@
       </c>
       <c r="L4" s="30"/>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>2</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>3</v>
       </c>
@@ -1387,7 +1390,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>4</v>
       </c>
@@ -1407,7 +1410,7 @@
         <v>77</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H7" s="26" t="s">
         <v>61</v>
@@ -1422,10 +1425,10 @@
         <v>39</v>
       </c>
       <c r="L7" s="48" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>5</v>
       </c>
@@ -1433,7 +1436,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>52</v>
@@ -1442,10 +1445,10 @@
         <v>3</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H8" s="26" t="s">
         <v>61</v>
@@ -1460,10 +1463,10 @@
         <v>39</v>
       </c>
       <c r="L8" s="29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="90" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>6</v>
       </c>
@@ -1471,7 +1474,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>52</v>
@@ -1483,7 +1486,7 @@
         <v>77</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H9" s="26" t="s">
         <v>61</v>
@@ -1498,10 +1501,10 @@
         <v>39</v>
       </c>
       <c r="L9" s="48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>7</v>
       </c>
@@ -1539,7 +1542,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>8</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>9</v>
       </c>
@@ -1612,10 +1615,10 @@
         <v>39</v>
       </c>
       <c r="L12" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>10</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>12</v>
       </c>
@@ -1691,7 +1694,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>13</v>
       </c>
@@ -1727,7 +1730,7 @@
       </c>
       <c r="L15" s="31"/>
     </row>
-    <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>14</v>
       </c>
@@ -1763,7 +1766,7 @@
       </c>
       <c r="L16" s="30"/>
     </row>
-    <row r="17" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>15</v>
       </c>
@@ -1799,7 +1802,7 @@
       </c>
       <c r="L17" s="30"/>
     </row>
-    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>16</v>
       </c>
@@ -1835,7 +1838,7 @@
       </c>
       <c r="L18" s="35"/>
     </row>
-    <row r="19" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>17</v>
       </c>
@@ -1869,11 +1872,11 @@
       <c r="K19" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L19" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>18</v>
       </c>
@@ -1907,11 +1910,11 @@
       <c r="K20" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="L20" s="30" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.3">
+      <c r="L20" s="29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>19</v>
       </c>
@@ -1945,9 +1948,9 @@
       <c r="K21" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="30"/>
-    </row>
-    <row r="22" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L21" s="29"/>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>20</v>
       </c>
@@ -1955,7 +1958,7 @@
         <v>15</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>12</v>
@@ -1981,9 +1984,9 @@
       <c r="K22" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="L22" s="30"/>
-    </row>
-    <row r="23" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L22" s="29"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>21</v>
       </c>
@@ -1991,7 +1994,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>12</v>
@@ -2000,7 +2003,7 @@
         <v>4</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G23" s="26" t="s">
         <v>86</v>
@@ -2017,45 +2020,45 @@
       <c r="K23" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="L23" s="30"/>
-    </row>
-    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.3">
+      <c r="L23" s="29"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>22</v>
       </c>
       <c r="B24" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="15" t="s">
+      <c r="D24" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="I24" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="38">
-        <v>14</v>
-      </c>
-      <c r="K24" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L24" s="30"/>
-    </row>
-    <row r="25" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I24" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="37">
+        <v>14</v>
+      </c>
+      <c r="K24" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L24" s="29"/>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>23</v>
       </c>
@@ -2063,7 +2066,7 @@
         <v>15</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>12</v>
@@ -2089,154 +2092,154 @@
       <c r="K25" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="L25" s="30"/>
-    </row>
-    <row r="26" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L25" s="29"/>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>24</v>
       </c>
       <c r="B26" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="15" t="s">
+      <c r="D26" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="33">
+        <v>4</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="I26" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K26" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L26" s="30"/>
-    </row>
-    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.3">
+      <c r="I26" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" s="53">
+        <v>14</v>
+      </c>
+      <c r="K26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="L26" s="35"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>25</v>
       </c>
       <c r="B27" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="15" t="s">
+      <c r="D27" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="33">
+        <v>3</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="I27" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K27" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L27" s="30"/>
+      <c r="I27" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27" s="53">
+        <v>14</v>
+      </c>
+      <c r="K27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="35"/>
       <c r="P27" s="57"/>
     </row>
-    <row r="28" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>26</v>
       </c>
       <c r="B28" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="39" t="s">
+      <c r="C28" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" s="15" t="s">
+      <c r="D28" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="33">
+        <v>3</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="I28" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K28" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L28" s="30"/>
-    </row>
-    <row r="29" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I28" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="J28" s="53">
+        <v>14</v>
+      </c>
+      <c r="K28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="L28" s="35"/>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>27</v>
       </c>
       <c r="B29" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="15" t="s">
+      <c r="D29" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="51">
+        <v>3</v>
+      </c>
+      <c r="F29" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="I29" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K29" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L29" s="30"/>
-    </row>
-    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.3">
+      <c r="I29" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="51">
+        <v>14</v>
+      </c>
+      <c r="K29" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29" s="61"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>28</v>
       </c>
@@ -2253,10 +2256,10 @@
         <v>4</v>
       </c>
       <c r="F30" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H30" s="37" t="s">
         <v>63</v>
@@ -2271,11 +2274,11 @@
         <v>39</v>
       </c>
       <c r="L30" s="29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="P30" s="57"/>
     </row>
-    <row r="31" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>29</v>
       </c>
@@ -2283,7 +2286,7 @@
         <v>21</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D31" s="54" t="s">
         <v>12</v>
@@ -2295,7 +2298,7 @@
         <v>86</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H31" s="37" t="s">
         <v>62</v>
@@ -2310,10 +2313,10 @@
         <v>39</v>
       </c>
       <c r="L31" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>30</v>
       </c>
@@ -2330,10 +2333,10 @@
         <v>3</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G32" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H32" s="37" t="s">
         <v>62</v>
@@ -2351,7 +2354,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>31</v>
       </c>
@@ -2359,7 +2362,7 @@
         <v>21</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D33" s="54" t="s">
         <v>12</v>
@@ -2368,10 +2371,10 @@
         <v>2</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G33" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H33" s="37" t="s">
         <v>62</v>
@@ -2386,10 +2389,10 @@
         <v>39</v>
       </c>
       <c r="L33" s="29" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>32</v>
       </c>
@@ -2425,7 +2428,7 @@
       </c>
       <c r="L34" s="30"/>
     </row>
-    <row r="35" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>33</v>
       </c>
@@ -2456,7 +2459,7 @@
       <c r="J35" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="66" t="s">
+      <c r="K35" s="58" t="s">
         <v>39</v>
       </c>
       <c r="L35" s="35"/>
@@ -2464,7 +2467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>34</v>
       </c>
@@ -2499,10 +2502,10 @@
         <v>39</v>
       </c>
       <c r="L36" s="29" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>35</v>
       </c>
@@ -2516,7 +2519,7 @@
         <v>12</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F37" s="26" t="s">
         <v>78</v>
@@ -2538,7 +2541,7 @@
       </c>
       <c r="L37" s="29"/>
     </row>
-    <row r="38" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
         <v>36</v>
       </c>
@@ -2552,7 +2555,7 @@
         <v>12</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F38" s="26" t="s">
         <v>86</v>
@@ -2573,10 +2576,10 @@
         <v>39</v>
       </c>
       <c r="L38" s="29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>37</v>
       </c>
@@ -2611,10 +2614,10 @@
         <v>39</v>
       </c>
       <c r="L39" s="29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <v>38</v>
       </c>
@@ -2653,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
         <v>39</v>
       </c>
@@ -2689,7 +2692,7 @@
       </c>
       <c r="L41" s="29"/>
     </row>
-    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>40</v>
       </c>
@@ -2703,7 +2706,7 @@
         <v>12</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F42" s="26" t="s">
         <v>77</v>
@@ -2724,10 +2727,10 @@
         <v>39</v>
       </c>
       <c r="L42" s="29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
         <v>41</v>
       </c>
@@ -2762,10 +2765,10 @@
         <v>39</v>
       </c>
       <c r="L43" s="29" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
         <v>42</v>
       </c>
@@ -2804,7 +2807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>43</v>
       </c>
@@ -2812,7 +2815,7 @@
         <v>21</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D45" s="25" t="s">
         <v>12</v>
@@ -2839,11 +2842,11 @@
         <v>39</v>
       </c>
       <c r="L45" s="48" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="N45" s="57"/>
     </row>
-    <row r="46" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>44</v>
       </c>
@@ -2851,7 +2854,7 @@
         <v>21</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D46" s="25" t="s">
         <v>12</v>
@@ -2878,10 +2881,10 @@
         <v>39</v>
       </c>
       <c r="L46" s="48" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
         <v>45</v>
       </c>
@@ -2889,7 +2892,7 @@
         <v>21</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D47" s="25" t="s">
         <v>12</v>
@@ -2916,10 +2919,10 @@
         <v>39</v>
       </c>
       <c r="L47" s="48" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>46</v>
       </c>
@@ -2927,7 +2930,7 @@
         <v>21</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D48" s="25" t="s">
         <v>12</v>
@@ -2954,10 +2957,10 @@
         <v>39</v>
       </c>
       <c r="L48" s="48" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
         <v>47</v>
       </c>
@@ -2965,7 +2968,7 @@
         <v>21</v>
       </c>
       <c r="C49" s="49" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D49" s="50" t="s">
         <v>12</v>
@@ -2996,7 +2999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="16"/>
       <c r="B50" s="18"/>
       <c r="C50" s="18"/>
@@ -3009,7 +3012,7 @@
       <c r="J50" s="18"/>
       <c r="K50" s="18"/>
     </row>
-    <row r="51" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>1</v>
       </c>
@@ -3042,7 +3045,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>2</v>
       </c>
@@ -3077,7 +3080,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>3</v>
       </c>
@@ -3112,7 +3115,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>4</v>
       </c>
@@ -3147,7 +3150,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
         <v>5</v>
       </c>
@@ -3182,7 +3185,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
         <v>6</v>
       </c>
@@ -3217,7 +3220,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
         <v>7</v>
       </c>
@@ -3252,7 +3255,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="16">
         <v>8</v>
       </c>
@@ -3287,7 +3290,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="16">
         <v>9</v>
       </c>
@@ -3322,7 +3325,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="16">
         <v>10</v>
       </c>
@@ -3357,7 +3360,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="16">
         <v>11</v>
       </c>
@@ -3392,7 +3395,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="16">
         <v>12</v>
       </c>
@@ -3427,7 +3430,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="16">
         <v>13</v>
       </c>
@@ -3462,7 +3465,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
         <v>14</v>
       </c>
@@ -3497,7 +3500,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="16">
         <v>15</v>
       </c>
@@ -3532,7 +3535,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="16">
         <v>16</v>
       </c>
@@ -3567,7 +3570,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="16">
         <v>17</v>
       </c>
@@ -3602,7 +3605,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="16">
         <v>18</v>
       </c>
@@ -3637,7 +3640,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="16">
         <v>19</v>
       </c>
@@ -3672,15 +3675,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C73" s="6"/>
       <c r="D73" s="7" t="s">
         <v>39</v>
@@ -3692,7 +3695,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C74" s="8" t="s">
         <v>61</v>
       </c>
@@ -3709,7 +3712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C75" s="8" t="s">
         <v>63</v>
       </c>
@@ -3726,7 +3729,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C76" s="8" t="s">
         <v>62</v>
       </c>
@@ -3743,13 +3746,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C79" s="9" t="s">
         <v>65</v>
       </c>
       <c r="D79" s="9">
         <f>COUNTIF(I4:I49,"To Do")</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E79" s="9">
         <f>COUNTIF(I52:I69,"To Do")</f>
@@ -3757,16 +3760,16 @@
       </c>
       <c r="F79" s="9">
         <f>SUM(E79,D79)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C80" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D80" s="9">
         <f>COUNTIF(I4:I49,"Doing")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E80" s="9">
         <f>COUNTIF(I52:I69,"Doing")</f>
@@ -3774,10 +3777,10 @@
       </c>
       <c r="F80" s="9">
         <f>SUM(D80,E80)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="3:6" ht="15" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C81" s="9" t="s">
         <v>67</v>
       </c>

</xml_diff>